<commit_message>
adding some more card details
</commit_message>
<xml_diff>
--- a/table-of-cards.xlsx
+++ b/table-of-cards.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\TopTrumps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\only1\Documents\GitHub\TopTrumps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AF4E793-E793-4324-BAD6-BFCA3B10B54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F69E311-D630-4E39-857F-0F833A9D2523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2955" yWindow="420" windowWidth="21945" windowHeight="13275" xr2:uid="{06C1F398-A751-40C7-BE85-AEF7567C634C}"/>
+    <workbookView xWindow="195" yWindow="255" windowWidth="12038" windowHeight="10013" xr2:uid="{06C1F398-A751-40C7-BE85-AEF7567C634C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>card number</t>
   </si>
@@ -106,6 +106,30 @@
   </si>
   <si>
     <t>spacer</t>
+  </si>
+  <si>
+    <t>100857.png</t>
+  </si>
+  <si>
+    <t>Fonio Millet</t>
+  </si>
+  <si>
+    <t>Hazelnut</t>
+  </si>
+  <si>
+    <t>Yellowhorn Tree</t>
+  </si>
+  <si>
+    <t>100877.png</t>
+  </si>
+  <si>
+    <t>100606.jpg</t>
+  </si>
+  <si>
+    <t>Pink Ipê Tree</t>
+  </si>
+  <si>
+    <t>100379.jpg</t>
   </si>
 </sst>
 </file>
@@ -457,26 +481,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9796A4-EDA2-43EE-A6FE-F13B61A291A2}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.73046875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -511,7 +536,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -540,11 +565,11 @@
         <v>17</v>
       </c>
       <c r="K2" t="str">
-        <f>CONCATENATE("const cards",A2," = new theCards('",B2,"', ",C2,", ",D2,", ",E2,", ",F2,", ",G2,", 'https://doi.org/10.5524/",H2,"' ,'./images/",I2,"');")</f>
+        <f t="shared" ref="K2:K13" si="0">CONCATENATE("const cards",A2," = new theCards('",B2,"', ",C2,", ",D2,", ",E2,", ",F2,", ",G2,", 'https://doi.org/10.5524/",H2,"' ,'./images/",I2,"');")</f>
         <v>const cards1 = new theCards('Darwins Finch', 2012.08, 1, 5, 284, 0.29, 'https://doi.org/10.5524/100040' ,'./images/100040.jpg');</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -573,11 +598,11 @@
         <v>18</v>
       </c>
       <c r="K3" t="str">
-        <f>CONCATENATE("const cards",A3," = new theCards('",B3,"', ",C3,", ",D3,", ",E3,", ",F3,", ",G3,", 'https://doi.org/10.5524/",H3,"' ,'./images/",I3,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards2 = new theCards('Puerto Rican Parrot', 2012.09, 1, 24, 568, 1.8, 'https://doi.org/10.5524/100039' ,'./images/100039.jpg');</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -606,11 +631,11 @@
         <v>19</v>
       </c>
       <c r="K4" t="str">
-        <f>CONCATENATE("const cards",A4," = new theCards('",B4,"', ",C4,", ",D4,", ",E4,", ",F4,", ",G4,", 'https://doi.org/10.5524/",H4,"' ,'./images/",I4,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards3 = new theCards('Pigeonpea', 2011.12, 1, 5, 157.6, 0.18, 'https://doi.org/10.5524/100028' ,'./images/100028.jpg');</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -639,11 +664,11 @@
         <v>20</v>
       </c>
       <c r="K5" t="str">
-        <f>CONCATENATE("const cards",A5," = new theCards('",B5,"', ",C5,", ",D5,", ",E5,", ",F5,", ",G5,", 'https://doi.org/10.5524/",H5,"' ,'./images/",I5,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards4 = new theCards('Crab-Eating Macaque', 2011.06, 1, 29, 1024, 2.4, 'https://doi.org/10.5524/100003' ,'./images/100003.jpg');</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -672,11 +697,11 @@
         <v>21</v>
       </c>
       <c r="K6" t="str">
-        <f>CONCATENATE("const cards",A6," = new theCards('",B6,"', ",C6,", ",D6,", ",E6,", ",F6,", ",G6,", 'https://doi.org/10.5524/",H6,"' ,'./images/",I6,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards5 = new theCards('Tibetan antelope', 2011.12, 1, 468, 2317, 232, 'https://doi.org/10.5524/100027' ,'./images/100027.jpg');</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -705,11 +730,11 @@
         <v>22</v>
       </c>
       <c r="K7" t="str">
-        <f>CONCATENATE("const cards",A7," = new theCards('",B7,"', ",C7,", ",D7,", ",E7,", ",F7,", ",G7,", 'https://doi.org/10.5524/",H7,"' ,'./images/",I7,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards6 = new theCards('Cucumber', 2011.12, 1, 16, 67, 0.76, 'https://doi.org/10.5524/100025' ,'./images/100025.jpg');</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -738,11 +763,11 @@
         <v>23</v>
       </c>
       <c r="K8" t="str">
-        <f>CONCATENATE("const cards",A8," = new theCards('",B8,"', ",C8,", ",D8,", ",E8,", ",F8,", ",G8,", 'https://doi.org/10.5524/",H8,"' ,'./images/",I8,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards7 = new theCards('Rhesus Macaque', 2011.06, 1, 10, 776, 0.98, 'https://doi.org/10.5524/100002' ,'./images/100002.jpg');</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -771,91 +796,294 @@
         <v>24</v>
       </c>
       <c r="K9" t="str">
-        <f>CONCATENATE("const cards",A9," = new theCards('",B9,"', ",C9,", ",D9,", ",E9,", ",F9,", ",G9,", 'https://doi.org/10.5524/",H9,"' ,'./images/",I9,"');")</f>
+        <f t="shared" si="0"/>
         <v>const cards8 = new theCards('Bald Eagle', 2014.05, 1, 5, 8.16, 384, 'https://doi.org/10.5524/101040' ,'./images/101040.png');</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>2021.01</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>48</v>
+      </c>
+      <c r="F10">
+        <v>6768</v>
+      </c>
+      <c r="G10">
+        <v>7.03</v>
+      </c>
+      <c r="H10">
+        <v>100857</v>
+      </c>
+      <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="0"/>
+        <v>const cards9 = new theCards('Fonio Millet', 2021.01, 1, 48, 6768, 7.03, 'https://doi.org/10.5524/100857' ,'./images/100857.png');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11">
+        <v>2021.03</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>35</v>
+      </c>
+      <c r="F11">
+        <v>353.56</v>
+      </c>
+      <c r="G11">
+        <v>1.21</v>
+      </c>
+      <c r="H11">
+        <v>100877</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="0"/>
+        <v>const cards10 = new theCards('Hazelnut', 2021.03, 2, 35, 353.56, 1.21, 'https://doi.org/10.5524/100877' ,'./images/100877.png');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>2019.03</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>35</v>
+      </c>
+      <c r="F12">
+        <v>485.86</v>
+      </c>
+      <c r="G12">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="H12">
+        <v>100606</v>
+      </c>
+      <c r="I12" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="0"/>
+        <v>const cards11 = new theCards('Yellowhorn Tree', 2019.03, 5, 35, 485.86, 2.24, 'https://doi.org/10.5524/100606' ,'./images/100606.jpg');</v>
+      </c>
+      <c r="L12">
+        <v>7776</v>
+      </c>
+      <c r="M12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <v>2017.11</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>16</v>
+      </c>
+      <c r="F13">
+        <v>140.1</v>
+      </c>
+      <c r="G13">
+        <v>0.2</v>
+      </c>
+      <c r="H13">
+        <v>100379</v>
+      </c>
+      <c r="I13" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="0"/>
+        <v>const cards12 = new theCards('Pink Ipê Tree', 2017.11, 2, 16, 140.1, 0.2, 'https://doi.org/10.5524/100379' ,'./images/100379.jpg');</v>
+      </c>
+      <c r="L13">
+        <v>991966016</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>116854</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>33971884</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>11801015</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>3786774</v>
+      </c>
+      <c r="M17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>22780139</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>256182</v>
+      </c>
+      <c r="M19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>589</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>6580680</v>
+      </c>
+      <c r="M21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>1333274198</v>
+      </c>
+      <c r="M22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
     </row>
+    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
+      <c r="L36">
+        <f>SUM(L12:L35)</f>
+        <v>2404542107</v>
+      </c>
+    </row>
+    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
+      <c r="L37">
+        <f>L36/1024</f>
+        <v>2348185.6513671875</v>
+      </c>
+    </row>
+    <row r="38" spans="12:12" x14ac:dyDescent="0.45">
+      <c r="L38">
+        <f>L37/1024</f>
+        <v>2293.150050163269</v>
+      </c>
+    </row>
+    <row r="39" spans="12:12" x14ac:dyDescent="0.45">
+      <c r="L39">
+        <f>L38/1024</f>
+        <v>2.2394043458625674</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>